<commit_message>
feat: new analysis files, including new data (2017 to 2019)
</commit_message>
<xml_diff>
--- a/src/main/results/analyses.xlsx
+++ b/src/main/results/analyses.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B6059D-435A-4F12-90C7-198B3819D64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,12 +146,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -179,7 +183,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -235,33 +238,38 @@
             <c:numRef>
               <c:f>Feuil1!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5583429</c:v>
+                  <c:v>5897965</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5782364</c:v>
+                  <c:v>6110595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5675068</c:v>
+                  <c:v>5998277</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5683564</c:v>
+                  <c:v>6006636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5702680</c:v>
+                  <c:v>6028839</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5008124</c:v>
+                  <c:v>5287820</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4576084</c:v>
+                  <c:v>4845189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4681-4AE7-8103-F7313265FC8B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -283,6 +291,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -302,7 +311,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standard" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -313,7 +322,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -329,7 +337,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -358,7 +366,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -429,48 +436,53 @@
             <c:numRef>
               <c:f>Feuil1!$B$11:$B$22</c:f>
               <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3132105</c:v>
+                  <c:v>3312169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2891141</c:v>
+                  <c:v>3050654</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3180480</c:v>
+                  <c:v>3352139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3157558</c:v>
+                  <c:v>3325769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3350212</c:v>
+                  <c:v>3533627</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3217603</c:v>
+                  <c:v>3397598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3364063</c:v>
+                  <c:v>3558635</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3212635</c:v>
+                  <c:v>3404147</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3147756</c:v>
+                  <c:v>3332798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3189325</c:v>
+                  <c:v>3379379</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3025796</c:v>
+                  <c:v>3205196</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3142639</c:v>
+                  <c:v>3323210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0166-4EFA-B502-572D66427597}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -492,6 +504,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -511,7 +524,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standard" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -522,7 +535,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -538,7 +550,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -581,7 +593,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -655,48 +666,52 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>101035.64516129032</c:v>
+                  <c:v>106844.16129032258</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102341.27433628318</c:v>
+                  <c:v>107987.75221238939</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102596.12903225806</c:v>
+                  <c:v>108133.51612903226</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105251.93333333333</c:v>
+                  <c:v>110858.96666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108071.35483870968</c:v>
+                  <c:v>113987.96774193548</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107253.43333333333</c:v>
+                  <c:v>113253.26666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>108518.16129032258</c:v>
+                  <c:v>114794.67741935483</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>103633.3870967742</c:v>
+                  <c:v>109811.19354838709</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104925.2</c:v>
+                  <c:v>111093.26666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>102881.45161290323</c:v>
+                  <c:v>109012.22580645161</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100859.86666666667</c:v>
+                  <c:v>106839.86666666667</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>101375.45161290323</c:v>
+                  <c:v>107200.32258064517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-013D-4D41-AFD2-A17863D9046C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -716,6 +731,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -757,7 +773,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -786,7 +802,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -814,10 +829,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$25:$A$73</c:f>
+              <c:f>Feuil1!$A$25:$A$76</c:f>
               <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>1968</c:v>
                 </c:pt>
@@ -964,16 +979,25 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$25:$B$73</c:f>
+              <c:f>Feuil1!$B$25:$B$76</c:f>
               <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>835796</c:v>
                 </c:pt>
@@ -1120,11 +1144,25 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>744697</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>730242</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>719737</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>714029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B363-43F9-9D38-CEC0E3A61FB8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1134,7 +1172,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="124582400"/>
         <c:axId val="125960192"/>
@@ -1146,7 +1183,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="Standard" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1165,7 +1202,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Standard" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1176,7 +1213,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1208,7 +1244,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1238,7 +1280,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1268,7 +1316,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Graphique 5"/>
+        <xdr:cNvPr id="6" name="Graphique 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1298,7 +1352,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Graphique 7"/>
+        <xdr:cNvPr id="8" name="Graphique 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1317,9 +1377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1357,7 +1417,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1429,7 +1489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1602,21 +1662,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,63 +1684,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5583429</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5897965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5782364</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6110595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5675068</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5998277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5683564</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6006636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5702680</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6028839</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5008124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5287820</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4576084</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4845189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1691,151 +1751,151 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>3132105</v>
+        <v>3312169</v>
       </c>
       <c r="C11" s="2">
         <f>B11/31</f>
-        <v>101035.64516129032</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>106844.16129032258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>2891141</v>
+        <v>3050654</v>
       </c>
       <c r="C12" s="2">
         <f>B12/28.25</f>
-        <v>102341.27433628318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>107987.75221238939</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3180480</v>
+        <v>3352139</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C12:C22" si="0">B13/31</f>
-        <v>102596.12903225806</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C13:C22" si="0">B13/31</f>
+        <v>108133.51612903226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>3157558</v>
+        <v>3325769</v>
       </c>
       <c r="C14" s="2">
         <f>B14/30</f>
-        <v>105251.93333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>110858.96666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>3350212</v>
+        <v>3533627</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>108071.35483870968</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>113987.96774193548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>3217603</v>
+        <v>3397598</v>
       </c>
       <c r="C16" s="2">
         <f>B16/30</f>
-        <v>107253.43333333333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>113253.26666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>3364063</v>
+        <v>3558635</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>108518.16129032258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>114794.67741935483</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>3212635</v>
+        <v>3404147</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>103633.3870967742</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109811.19354838709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>3147756</v>
+        <v>3332798</v>
       </c>
       <c r="C19" s="2">
         <f>B19/30</f>
-        <v>104925.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>111093.26666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>3189325</v>
+        <v>3379379</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>102881.45161290323</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109012.22580645161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>3025796</v>
+        <v>3205196</v>
       </c>
       <c r="C21" s="2">
         <f>B21/30</f>
-        <v>100859.86666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>106839.86666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>3142639</v>
+        <v>3323210</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>101375.45161290323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>107200.32258064517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1843,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>1968</v>
       </c>
@@ -1851,7 +1911,7 @@
         <v>835796</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1969</v>
       </c>
@@ -1859,7 +1919,7 @@
         <v>842245</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>1970</v>
       </c>
@@ -1867,7 +1927,7 @@
         <v>850381</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1971</v>
       </c>
@@ -1875,7 +1935,7 @@
         <v>881284</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1972</v>
       </c>
@@ -1883,7 +1943,7 @@
         <v>877506</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1973</v>
       </c>
@@ -1891,7 +1951,7 @@
         <v>857186</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>1974</v>
       </c>
@@ -1899,7 +1959,7 @@
         <v>801218</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>1975</v>
       </c>
@@ -1907,7 +1967,7 @@
         <v>745065</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>1976</v>
       </c>
@@ -1915,7 +1975,7 @@
         <v>720395</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>1977</v>
       </c>
@@ -1923,7 +1983,7 @@
         <v>744744</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>1978</v>
       </c>
@@ -1931,7 +1991,7 @@
         <v>737062</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>1979</v>
       </c>
@@ -1939,7 +1999,7 @@
         <v>757354</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>1980</v>
       </c>
@@ -1947,7 +2007,7 @@
         <v>800376</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>1981</v>
       </c>
@@ -1955,7 +2015,7 @@
         <v>805483</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>1982</v>
       </c>
@@ -1963,7 +2023,7 @@
         <v>797223</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>1983</v>
       </c>
@@ -1971,7 +2031,7 @@
         <v>748525</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>1984</v>
       </c>
@@ -1979,7 +2039,7 @@
         <v>759939</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>1985</v>
       </c>
@@ -1987,7 +2047,7 @@
         <v>768431</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>1986</v>
       </c>
@@ -1995,7 +2055,7 @@
         <v>778468</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>1987</v>
       </c>
@@ -2003,7 +2063,7 @@
         <v>767828</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -2011,7 +2071,7 @@
         <v>771268</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>1989</v>
       </c>
@@ -2019,7 +2079,7 @@
         <v>765473</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -2027,7 +2087,7 @@
         <v>762407</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>1991</v>
       </c>
@@ -2035,7 +2095,7 @@
         <v>759056</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>1992</v>
       </c>
@@ -2043,7 +2103,7 @@
         <v>743658</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -2051,7 +2111,7 @@
         <v>711610</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>1994</v>
       </c>
@@ -2059,7 +2119,7 @@
         <v>710993</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>1995</v>
       </c>
@@ -2067,7 +2127,7 @@
         <v>729609</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>1996</v>
       </c>
@@ -2075,7 +2135,7 @@
         <v>734338</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>1997</v>
       </c>
@@ -2083,7 +2143,7 @@
         <v>726768</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>1998</v>
       </c>
@@ -2091,7 +2151,7 @@
         <v>738080</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -2099,7 +2159,7 @@
         <v>744791</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>2000</v>
       </c>
@@ -2107,7 +2167,7 @@
         <v>774782</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>2001</v>
       </c>
@@ -2115,7 +2175,7 @@
         <v>770945</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>2002</v>
       </c>
@@ -2123,7 +2183,7 @@
         <v>761630</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>2003</v>
       </c>
@@ -2131,7 +2191,7 @@
         <v>761464</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>2004</v>
       </c>
@@ -2139,7 +2199,7 @@
         <v>767816</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>2005</v>
       </c>
@@ -2147,7 +2207,7 @@
         <v>774355</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>2006</v>
       </c>
@@ -2155,7 +2215,7 @@
         <v>796896</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -2163,7 +2223,7 @@
         <v>785985</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -2171,7 +2231,7 @@
         <v>796044</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>2009</v>
       </c>
@@ -2179,7 +2239,7 @@
         <v>793420</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>2010</v>
       </c>
@@ -2187,7 +2247,7 @@
         <v>802224</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -2195,7 +2255,7 @@
         <v>792996</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>2012</v>
       </c>
@@ -2203,7 +2263,7 @@
         <v>790290</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>2013</v>
       </c>
@@ -2211,7 +2271,7 @@
         <v>781621</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>2014</v>
       </c>
@@ -2219,7 +2279,7 @@
         <v>781167</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>2015</v>
       </c>
@@ -2227,12 +2287,36 @@
         <v>760421</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>2016</v>
       </c>
       <c r="B73">
         <v>744697</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>2017</v>
+      </c>
+      <c r="B74">
+        <v>730242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>2018</v>
+      </c>
+      <c r="B75">
+        <v>719737</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>2019</v>
+      </c>
+      <c r="B76">
+        <v>714029</v>
       </c>
     </row>
   </sheetData>
@@ -2243,24 +2327,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>